<commit_message>
pii for some apps
</commit_message>
<xml_diff>
--- a/mitm/curated/apps and pii.xlsx
+++ b/mitm/curated/apps and pii.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="460" windowWidth="25000" windowHeight="14660" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="24060" windowHeight="14540" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="apps preselection" sheetId="1" r:id="rId1"/>
-    <sheet name="selected apps" sheetId="2" r:id="rId2"/>
+    <sheet name="apps and PII" sheetId="3" r:id="rId1"/>
+    <sheet name="apps preselection" sheetId="1" r:id="rId2"/>
+    <sheet name="selected apps" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="101">
   <si>
     <t>Pokemon</t>
   </si>
@@ -199,13 +200,145 @@
   </si>
   <si>
     <t>Top goole store</t>
+  </si>
+  <si>
+    <t>first party</t>
+  </si>
+  <si>
+    <t>third party</t>
+  </si>
+  <si>
+    <t>PII</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>google.com</t>
+  </si>
+  <si>
+    <t>yes (GB)</t>
+  </si>
+  <si>
+    <t>Domains</t>
+  </si>
+  <si>
+    <t>Organisations</t>
+  </si>
+  <si>
+    <t>http://m.me</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Facebook Inc.</t>
+  </si>
+  <si>
+    <t>Google.com// akamaihd.net</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>akamaihd.net</t>
+  </si>
+  <si>
+    <t>Akamai</t>
+  </si>
+  <si>
+    <t>Video//cloud</t>
+  </si>
+  <si>
+    <t>us</t>
+  </si>
+  <si>
+    <t>Data from Havard (cannot be proxied)</t>
+  </si>
+  <si>
+    <t>But nothing was found on iOS</t>
+  </si>
+  <si>
+    <t>Google (google.com;googleapis.com)//Microsoft (msn.com:443)</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Phone no.</t>
+  </si>
+  <si>
+    <t>Fields not included</t>
+  </si>
+  <si>
+    <t>Birthday</t>
+  </si>
+  <si>
+    <t>not sure this can be replicated</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>same above and it's more security than privacy</t>
+  </si>
+  <si>
+    <t>Employment</t>
+  </si>
+  <si>
+    <t>specialised apps (not applicable to those we studied)</t>
+  </si>
+  <si>
+    <t>Friend</t>
+  </si>
+  <si>
+    <t>Not sensitive</t>
+  </si>
+  <si>
+    <t>Medical info</t>
+  </si>
+  <si>
+    <t>Behaviours (post/search)</t>
+  </si>
+  <si>
+    <t>Not PII</t>
+  </si>
+  <si>
+    <t>Postcoede</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>google(android)//paypal(ios)</t>
+  </si>
+  <si>
+    <t>crittercism//facebook//flurry//google//twitter(android)//yoz.io(ios)</t>
+  </si>
+  <si>
+    <t>appspot.com//facebook.com(android)</t>
+  </si>
+  <si>
+    <t>google (android)//yanooapis.com(ios)//facebook(ios)//apple.com(ios)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -244,8 +377,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -258,8 +403,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -267,13 +418,94 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -283,10 +515,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -562,6 +808,456 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="3"/>
+    <col min="2" max="2" width="19.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" style="3" customWidth="1"/>
+    <col min="5" max="13" width="10.83203125" style="3"/>
+    <col min="14" max="14" width="28.1640625" style="3" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="N2" s="7"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="G9" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B10" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B12" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="O17" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13"/>
+      <c r="S17" s="14"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O18" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="P18" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="16"/>
+      <c r="S18" s="17"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O19" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="P19" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="16"/>
+      <c r="S19" s="17"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O20" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="P20" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="17"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="O21" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="P21" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q21" s="16"/>
+      <c r="R21" s="16"/>
+      <c r="S21" s="17"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B22" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="O22" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="P22" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q22" s="16"/>
+      <c r="R22" s="16"/>
+      <c r="S22" s="17"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B23" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="O23" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="P23" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q23" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="R23" s="19"/>
+      <c r="S23" s="20"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S30" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="O7" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1027,11 +1723,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>